<commit_message>
ANS-006-150 - Gestion des identifiants métiers (#381)
* Commit system

* maj system

* Fix PR

* Harmonisation des noms de fichiers d857ffafc2039b1f682766b53ed616c63ef79a47
</commit_message>
<xml_diff>
--- a/main/ig/StructureDefinition-tddui-encounter-sejour.xlsx
+++ b/main/ig/StructureDefinition-tddui-encounter-sejour.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3451" uniqueCount="594">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3451" uniqueCount="595">
   <si>
     <t>Property</t>
   </si>
@@ -57,7 +57,7 @@
     <t>Date</t>
   </si>
   <si>
-    <t>2025-10-20T13:54:58+00:00</t>
+    <t>2025-10-23T09:18:35+00:00</t>
   </si>
   <si>
     <t>Publisher</t>
@@ -777,6 +777,9 @@
   </si>
   <si>
     <t>There are many sets  of identifiers.  To perform matching of two identifiers, we need to know what set we're dealing with. The system identifies a particular set of unique identifiers.</t>
+  </si>
+  <si>
+    <t>https://identifiant-medicosocial-sejour.esante.gouv.fr</t>
   </si>
   <si>
     <t>http://www.acme.com/identifiers/patient</t>
@@ -4806,7 +4809,7 @@
       </c>
       <c r="E23" s="2"/>
       <c r="F23" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G23" t="s" s="2">
         <v>90</v>
@@ -4843,10 +4846,10 @@
         <v>81</v>
       </c>
       <c r="S23" t="s" s="2">
-        <v>81</v>
+        <v>242</v>
       </c>
       <c r="T23" t="s" s="2">
-        <v>242</v>
+        <v>243</v>
       </c>
       <c r="U23" t="s" s="2">
         <v>81</v>
@@ -4882,7 +4885,7 @@
         <v>81</v>
       </c>
       <c r="AF23" t="s" s="2">
-        <v>243</v>
+        <v>244</v>
       </c>
       <c r="AG23" t="s" s="2">
         <v>79</v>
@@ -4903,21 +4906,21 @@
         <v>81</v>
       </c>
       <c r="AM23" t="s" s="2">
-        <v>244</v>
+        <v>245</v>
       </c>
       <c r="AN23" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO23" t="s" s="2">
-        <v>245</v>
+        <v>246</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="s" s="2">
-        <v>246</v>
+        <v>247</v>
       </c>
       <c r="B24" t="s" s="2">
-        <v>247</v>
+        <v>248</v>
       </c>
       <c r="C24" s="2"/>
       <c r="D24" t="s" s="2">
@@ -4925,7 +4928,7 @@
       </c>
       <c r="E24" s="2"/>
       <c r="F24" t="s" s="2">
-        <v>79</v>
+        <v>90</v>
       </c>
       <c r="G24" t="s" s="2">
         <v>90</v>
@@ -4943,13 +4946,13 @@
         <v>201</v>
       </c>
       <c r="L24" t="s" s="2">
-        <v>248</v>
+        <v>249</v>
       </c>
       <c r="M24" t="s" s="2">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="N24" t="s" s="2">
-        <v>250</v>
+        <v>251</v>
       </c>
       <c r="O24" s="2"/>
       <c r="P24" t="s" s="2">
@@ -4963,7 +4966,7 @@
         <v>81</v>
       </c>
       <c r="T24" t="s" s="2">
-        <v>251</v>
+        <v>252</v>
       </c>
       <c r="U24" t="s" s="2">
         <v>81</v>
@@ -4999,7 +5002,7 @@
         <v>81</v>
       </c>
       <c r="AF24" t="s" s="2">
-        <v>252</v>
+        <v>253</v>
       </c>
       <c r="AG24" t="s" s="2">
         <v>79</v>
@@ -5020,21 +5023,21 @@
         <v>81</v>
       </c>
       <c r="AM24" t="s" s="2">
-        <v>253</v>
+        <v>254</v>
       </c>
       <c r="AN24" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO24" t="s" s="2">
-        <v>254</v>
+        <v>255</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="s" s="2">
-        <v>255</v>
+        <v>256</v>
       </c>
       <c r="B25" t="s" s="2">
-        <v>256</v>
+        <v>257</v>
       </c>
       <c r="C25" s="2"/>
       <c r="D25" t="s" s="2">
@@ -5057,13 +5060,13 @@
         <v>91</v>
       </c>
       <c r="K25" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L25" t="s" s="2">
-        <v>258</v>
+        <v>259</v>
       </c>
       <c r="M25" t="s" s="2">
-        <v>259</v>
+        <v>260</v>
       </c>
       <c r="N25" s="2"/>
       <c r="O25" s="2"/>
@@ -5114,7 +5117,7 @@
         <v>81</v>
       </c>
       <c r="AF25" t="s" s="2">
-        <v>260</v>
+        <v>261</v>
       </c>
       <c r="AG25" t="s" s="2">
         <v>79</v>
@@ -5135,21 +5138,21 @@
         <v>81</v>
       </c>
       <c r="AM25" t="s" s="2">
-        <v>261</v>
+        <v>262</v>
       </c>
       <c r="AN25" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO25" t="s" s="2">
-        <v>262</v>
+        <v>263</v>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="s" s="2">
-        <v>263</v>
+        <v>264</v>
       </c>
       <c r="B26" t="s" s="2">
-        <v>264</v>
+        <v>265</v>
       </c>
       <c r="C26" s="2"/>
       <c r="D26" t="s" s="2">
@@ -5172,16 +5175,16 @@
         <v>91</v>
       </c>
       <c r="K26" t="s" s="2">
-        <v>265</v>
+        <v>266</v>
       </c>
       <c r="L26" t="s" s="2">
-        <v>266</v>
+        <v>267</v>
       </c>
       <c r="M26" t="s" s="2">
-        <v>267</v>
+        <v>268</v>
       </c>
       <c r="N26" t="s" s="2">
-        <v>268</v>
+        <v>269</v>
       </c>
       <c r="O26" s="2"/>
       <c r="P26" t="s" s="2">
@@ -5231,7 +5234,7 @@
         <v>81</v>
       </c>
       <c r="AF26" t="s" s="2">
-        <v>269</v>
+        <v>270</v>
       </c>
       <c r="AG26" t="s" s="2">
         <v>79</v>
@@ -5252,21 +5255,21 @@
         <v>81</v>
       </c>
       <c r="AM26" t="s" s="2">
-        <v>270</v>
+        <v>271</v>
       </c>
       <c r="AN26" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO26" t="s" s="2">
-        <v>271</v>
+        <v>272</v>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="B27" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="C27" s="2"/>
       <c r="D27" t="s" s="2">
@@ -5292,13 +5295,13 @@
         <v>110</v>
       </c>
       <c r="L27" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="M27" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="N27" t="s" s="2">
-        <v>275</v>
+        <v>276</v>
       </c>
       <c r="O27" s="2"/>
       <c r="P27" t="s" s="2">
@@ -5327,10 +5330,10 @@
         <v>218</v>
       </c>
       <c r="Y27" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="Z27" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AA27" t="s" s="2">
         <v>81</v>
@@ -5348,7 +5351,7 @@
         <v>81</v>
       </c>
       <c r="AF27" t="s" s="2">
-        <v>272</v>
+        <v>273</v>
       </c>
       <c r="AG27" t="s" s="2">
         <v>90</v>
@@ -5366,24 +5369,24 @@
         <v>81</v>
       </c>
       <c r="AL27" t="s" s="2">
-        <v>278</v>
+        <v>279</v>
       </c>
       <c r="AM27" t="s" s="2">
-        <v>279</v>
+        <v>280</v>
       </c>
       <c r="AN27" t="s" s="2">
-        <v>280</v>
+        <v>281</v>
       </c>
       <c r="AO27" t="s" s="2">
-        <v>281</v>
+        <v>282</v>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="B28" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="C28" s="2"/>
       <c r="D28" t="s" s="2">
@@ -5406,16 +5409,16 @@
         <v>81</v>
       </c>
       <c r="K28" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L28" t="s" s="2">
-        <v>284</v>
+        <v>285</v>
       </c>
       <c r="M28" t="s" s="2">
-        <v>285</v>
+        <v>286</v>
       </c>
       <c r="N28" t="s" s="2">
-        <v>286</v>
+        <v>287</v>
       </c>
       <c r="O28" s="2"/>
       <c r="P28" t="s" s="2">
@@ -5465,7 +5468,7 @@
         <v>81</v>
       </c>
       <c r="AF28" t="s" s="2">
-        <v>282</v>
+        <v>283</v>
       </c>
       <c r="AG28" t="s" s="2">
         <v>79</v>
@@ -5497,10 +5500,10 @@
     </row>
     <row r="29">
       <c r="A29" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="B29" t="s" s="2">
-        <v>287</v>
+        <v>288</v>
       </c>
       <c r="C29" s="2"/>
       <c r="D29" t="s" s="2">
@@ -5612,10 +5615,10 @@
     </row>
     <row r="30">
       <c r="A30" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="B30" t="s" s="2">
-        <v>288</v>
+        <v>289</v>
       </c>
       <c r="C30" s="2"/>
       <c r="D30" t="s" s="2">
@@ -5729,14 +5732,14 @@
     </row>
     <row r="31">
       <c r="A31" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="B31" t="s" s="2">
-        <v>289</v>
+        <v>290</v>
       </c>
       <c r="C31" s="2"/>
       <c r="D31" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E31" s="2"/>
       <c r="F31" t="s" s="2">
@@ -5758,10 +5761,10 @@
         <v>135</v>
       </c>
       <c r="L31" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M31" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N31" t="s" s="2">
         <v>183</v>
@@ -5816,7 +5819,7 @@
         <v>81</v>
       </c>
       <c r="AF31" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG31" t="s" s="2">
         <v>79</v>
@@ -5848,10 +5851,10 @@
     </row>
     <row r="32">
       <c r="A32" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="B32" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="C32" s="2"/>
       <c r="D32" t="s" s="2">
@@ -5877,10 +5880,10 @@
         <v>110</v>
       </c>
       <c r="L32" t="s" s="2">
-        <v>273</v>
+        <v>274</v>
       </c>
       <c r="M32" t="s" s="2">
-        <v>274</v>
+        <v>275</v>
       </c>
       <c r="N32" s="2"/>
       <c r="O32" s="2"/>
@@ -5910,10 +5913,10 @@
         <v>218</v>
       </c>
       <c r="Y32" t="s" s="2">
-        <v>276</v>
+        <v>277</v>
       </c>
       <c r="Z32" t="s" s="2">
-        <v>277</v>
+        <v>278</v>
       </c>
       <c r="AA32" t="s" s="2">
         <v>81</v>
@@ -5931,7 +5934,7 @@
         <v>81</v>
       </c>
       <c r="AF32" t="s" s="2">
-        <v>294</v>
+        <v>295</v>
       </c>
       <c r="AG32" t="s" s="2">
         <v>90</v>
@@ -5963,10 +5966,10 @@
     </row>
     <row r="33">
       <c r="A33" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="B33" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="C33" s="2"/>
       <c r="D33" t="s" s="2">
@@ -5989,13 +5992,13 @@
         <v>81</v>
       </c>
       <c r="K33" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L33" t="s" s="2">
-        <v>296</v>
+        <v>297</v>
       </c>
       <c r="M33" t="s" s="2">
-        <v>297</v>
+        <v>298</v>
       </c>
       <c r="N33" s="2"/>
       <c r="O33" s="2"/>
@@ -6046,7 +6049,7 @@
         <v>81</v>
       </c>
       <c r="AF33" t="s" s="2">
-        <v>295</v>
+        <v>296</v>
       </c>
       <c r="AG33" t="s" s="2">
         <v>90</v>
@@ -6078,10 +6081,10 @@
     </row>
     <row r="34">
       <c r="A34" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="B34" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="C34" s="2"/>
       <c r="D34" t="s" s="2">
@@ -6104,13 +6107,13 @@
         <v>91</v>
       </c>
       <c r="K34" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L34" t="s" s="2">
-        <v>300</v>
+        <v>301</v>
       </c>
       <c r="M34" t="s" s="2">
-        <v>301</v>
+        <v>302</v>
       </c>
       <c r="N34" s="2"/>
       <c r="O34" s="2"/>
@@ -6140,10 +6143,10 @@
         <v>231</v>
       </c>
       <c r="Y34" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="Z34" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AA34" t="s" s="2">
         <v>81</v>
@@ -6161,7 +6164,7 @@
         <v>81</v>
       </c>
       <c r="AF34" t="s" s="2">
-        <v>298</v>
+        <v>299</v>
       </c>
       <c r="AG34" t="s" s="2">
         <v>90</v>
@@ -6182,21 +6185,21 @@
         <v>81</v>
       </c>
       <c r="AM34" t="s" s="2">
-        <v>304</v>
+        <v>305</v>
       </c>
       <c r="AN34" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AO34" t="s" s="2">
-        <v>306</v>
+        <v>307</v>
       </c>
     </row>
     <row r="35">
       <c r="A35" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="B35" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="C35" s="2"/>
       <c r="D35" t="s" s="2">
@@ -6219,13 +6222,13 @@
         <v>81</v>
       </c>
       <c r="K35" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L35" t="s" s="2">
-        <v>308</v>
+        <v>309</v>
       </c>
       <c r="M35" t="s" s="2">
-        <v>309</v>
+        <v>310</v>
       </c>
       <c r="N35" s="2"/>
       <c r="O35" s="2"/>
@@ -6276,7 +6279,7 @@
         <v>81</v>
       </c>
       <c r="AF35" t="s" s="2">
-        <v>307</v>
+        <v>308</v>
       </c>
       <c r="AG35" t="s" s="2">
         <v>79</v>
@@ -6308,10 +6311,10 @@
     </row>
     <row r="36">
       <c r="A36" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="B36" t="s" s="2">
-        <v>310</v>
+        <v>311</v>
       </c>
       <c r="C36" s="2"/>
       <c r="D36" t="s" s="2">
@@ -6423,10 +6426,10 @@
     </row>
     <row r="37">
       <c r="A37" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="B37" t="s" s="2">
-        <v>311</v>
+        <v>312</v>
       </c>
       <c r="C37" s="2"/>
       <c r="D37" t="s" s="2">
@@ -6540,14 +6543,14 @@
     </row>
     <row r="38">
       <c r="A38" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="B38" t="s" s="2">
-        <v>312</v>
+        <v>313</v>
       </c>
       <c r="C38" s="2"/>
       <c r="D38" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E38" s="2"/>
       <c r="F38" t="s" s="2">
@@ -6569,10 +6572,10 @@
         <v>135</v>
       </c>
       <c r="L38" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M38" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N38" t="s" s="2">
         <v>183</v>
@@ -6627,7 +6630,7 @@
         <v>81</v>
       </c>
       <c r="AF38" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG38" t="s" s="2">
         <v>79</v>
@@ -6659,10 +6662,10 @@
     </row>
     <row r="39">
       <c r="A39" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="B39" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="C39" s="2"/>
       <c r="D39" t="s" s="2">
@@ -6685,13 +6688,13 @@
         <v>81</v>
       </c>
       <c r="K39" t="s" s="2">
-        <v>299</v>
+        <v>300</v>
       </c>
       <c r="L39" t="s" s="2">
-        <v>314</v>
+        <v>315</v>
       </c>
       <c r="M39" t="s" s="2">
-        <v>315</v>
+        <v>316</v>
       </c>
       <c r="N39" s="2"/>
       <c r="O39" s="2"/>
@@ -6721,10 +6724,10 @@
         <v>231</v>
       </c>
       <c r="Y39" t="s" s="2">
-        <v>302</v>
+        <v>303</v>
       </c>
       <c r="Z39" t="s" s="2">
-        <v>303</v>
+        <v>304</v>
       </c>
       <c r="AA39" t="s" s="2">
         <v>81</v>
@@ -6742,7 +6745,7 @@
         <v>81</v>
       </c>
       <c r="AF39" t="s" s="2">
-        <v>313</v>
+        <v>314</v>
       </c>
       <c r="AG39" t="s" s="2">
         <v>90</v>
@@ -6774,10 +6777,10 @@
     </row>
     <row r="40">
       <c r="A40" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="B40" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="C40" s="2"/>
       <c r="D40" t="s" s="2">
@@ -6800,13 +6803,13 @@
         <v>81</v>
       </c>
       <c r="K40" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L40" t="s" s="2">
-        <v>317</v>
+        <v>318</v>
       </c>
       <c r="M40" t="s" s="2">
-        <v>318</v>
+        <v>319</v>
       </c>
       <c r="N40" s="2"/>
       <c r="O40" s="2"/>
@@ -6857,7 +6860,7 @@
         <v>81</v>
       </c>
       <c r="AF40" t="s" s="2">
-        <v>316</v>
+        <v>317</v>
       </c>
       <c r="AG40" t="s" s="2">
         <v>90</v>
@@ -6889,10 +6892,10 @@
     </row>
     <row r="41">
       <c r="A41" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="B41" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="C41" s="2"/>
       <c r="D41" t="s" s="2">
@@ -6918,13 +6921,13 @@
         <v>225</v>
       </c>
       <c r="L41" t="s" s="2">
-        <v>320</v>
+        <v>321</v>
       </c>
       <c r="M41" t="s" s="2">
-        <v>321</v>
+        <v>322</v>
       </c>
       <c r="N41" t="s" s="2">
-        <v>322</v>
+        <v>323</v>
       </c>
       <c r="O41" s="2"/>
       <c r="P41" t="s" s="2">
@@ -6950,13 +6953,13 @@
         <v>81</v>
       </c>
       <c r="X41" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Y41" t="s" s="2">
-        <v>324</v>
+        <v>325</v>
       </c>
       <c r="Z41" t="s" s="2">
-        <v>325</v>
+        <v>326</v>
       </c>
       <c r="AA41" t="s" s="2">
         <v>81</v>
@@ -6974,7 +6977,7 @@
         <v>81</v>
       </c>
       <c r="AF41" t="s" s="2">
-        <v>319</v>
+        <v>320</v>
       </c>
       <c r="AG41" t="s" s="2">
         <v>79</v>
@@ -6992,24 +6995,24 @@
         <v>81</v>
       </c>
       <c r="AL41" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AM41" t="s" s="2">
-        <v>327</v>
+        <v>328</v>
       </c>
       <c r="AN41" t="s" s="2">
-        <v>305</v>
+        <v>306</v>
       </c>
       <c r="AO41" t="s" s="2">
-        <v>328</v>
+        <v>329</v>
       </c>
     </row>
     <row r="42">
       <c r="A42" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="B42" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="C42" s="2"/>
       <c r="D42" t="s" s="2">
@@ -7035,10 +7038,10 @@
         <v>225</v>
       </c>
       <c r="L42" t="s" s="2">
-        <v>330</v>
+        <v>331</v>
       </c>
       <c r="M42" t="s" s="2">
-        <v>331</v>
+        <v>332</v>
       </c>
       <c r="N42" s="2"/>
       <c r="O42" s="2"/>
@@ -7065,13 +7068,13 @@
         <v>81</v>
       </c>
       <c r="X42" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Y42" t="s" s="2">
-        <v>332</v>
+        <v>333</v>
       </c>
       <c r="Z42" t="s" s="2">
-        <v>333</v>
+        <v>334</v>
       </c>
       <c r="AA42" t="s" s="2">
         <v>81</v>
@@ -7089,7 +7092,7 @@
         <v>81</v>
       </c>
       <c r="AF42" t="s" s="2">
-        <v>329</v>
+        <v>330</v>
       </c>
       <c r="AG42" t="s" s="2">
         <v>79</v>
@@ -7107,7 +7110,7 @@
         <v>81</v>
       </c>
       <c r="AL42" t="s" s="2">
-        <v>326</v>
+        <v>327</v>
       </c>
       <c r="AM42" t="s" s="2">
         <v>205</v>
@@ -7116,15 +7119,15 @@
         <v>81</v>
       </c>
       <c r="AO42" t="s" s="2">
-        <v>334</v>
+        <v>335</v>
       </c>
     </row>
     <row r="43">
       <c r="A43" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="B43" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="C43" s="2"/>
       <c r="D43" t="s" s="2">
@@ -7150,10 +7153,10 @@
         <v>225</v>
       </c>
       <c r="L43" t="s" s="2">
-        <v>336</v>
+        <v>337</v>
       </c>
       <c r="M43" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="N43" s="2"/>
       <c r="O43" s="2"/>
@@ -7180,13 +7183,13 @@
         <v>81</v>
       </c>
       <c r="X43" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Y43" t="s" s="2">
-        <v>337</v>
+        <v>338</v>
       </c>
       <c r="Z43" t="s" s="2">
-        <v>338</v>
+        <v>339</v>
       </c>
       <c r="AA43" t="s" s="2">
         <v>81</v>
@@ -7204,7 +7207,7 @@
         <v>81</v>
       </c>
       <c r="AF43" t="s" s="2">
-        <v>335</v>
+        <v>336</v>
       </c>
       <c r="AG43" t="s" s="2">
         <v>79</v>
@@ -7225,25 +7228,25 @@
         <v>81</v>
       </c>
       <c r="AM43" t="s" s="2">
-        <v>339</v>
+        <v>340</v>
       </c>
       <c r="AN43" t="s" s="2">
-        <v>340</v>
+        <v>341</v>
       </c>
       <c r="AO43" t="s" s="2">
-        <v>341</v>
+        <v>342</v>
       </c>
     </row>
     <row r="44">
       <c r="A44" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="B44" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="C44" s="2"/>
       <c r="D44" t="s" s="2">
-        <v>343</v>
+        <v>344</v>
       </c>
       <c r="E44" s="2"/>
       <c r="F44" t="s" s="2">
@@ -7262,16 +7265,16 @@
         <v>91</v>
       </c>
       <c r="K44" t="s" s="2">
-        <v>344</v>
+        <v>345</v>
       </c>
       <c r="L44" t="s" s="2">
-        <v>345</v>
+        <v>346</v>
       </c>
       <c r="M44" t="s" s="2">
-        <v>346</v>
+        <v>347</v>
       </c>
       <c r="N44" t="s" s="2">
-        <v>347</v>
+        <v>348</v>
       </c>
       <c r="O44" s="2"/>
       <c r="P44" t="s" s="2">
@@ -7321,7 +7324,7 @@
         <v>81</v>
       </c>
       <c r="AF44" t="s" s="2">
-        <v>342</v>
+        <v>343</v>
       </c>
       <c r="AG44" t="s" s="2">
         <v>79</v>
@@ -7336,27 +7339,27 @@
         <v>102</v>
       </c>
       <c r="AK44" t="s" s="2">
-        <v>348</v>
+        <v>349</v>
       </c>
       <c r="AL44" t="s" s="2">
-        <v>349</v>
+        <v>350</v>
       </c>
       <c r="AM44" t="s" s="2">
-        <v>350</v>
+        <v>351</v>
       </c>
       <c r="AN44" t="s" s="2">
-        <v>351</v>
+        <v>352</v>
       </c>
       <c r="AO44" t="s" s="2">
-        <v>352</v>
+        <v>353</v>
       </c>
     </row>
     <row r="45">
       <c r="A45" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="B45" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="C45" s="2"/>
       <c r="D45" t="s" s="2">
@@ -7379,13 +7382,13 @@
         <v>91</v>
       </c>
       <c r="K45" t="s" s="2">
-        <v>354</v>
+        <v>355</v>
       </c>
       <c r="L45" t="s" s="2">
-        <v>355</v>
+        <v>356</v>
       </c>
       <c r="M45" t="s" s="2">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="N45" s="2"/>
       <c r="O45" s="2"/>
@@ -7436,7 +7439,7 @@
         <v>81</v>
       </c>
       <c r="AF45" t="s" s="2">
-        <v>353</v>
+        <v>354</v>
       </c>
       <c r="AG45" t="s" s="2">
         <v>79</v>
@@ -7454,28 +7457,28 @@
         <v>81</v>
       </c>
       <c r="AL45" t="s" s="2">
-        <v>357</v>
+        <v>358</v>
       </c>
       <c r="AM45" t="s" s="2">
         <v>205</v>
       </c>
       <c r="AN45" t="s" s="2">
-        <v>358</v>
+        <v>359</v>
       </c>
       <c r="AO45" t="s" s="2">
-        <v>359</v>
+        <v>360</v>
       </c>
     </row>
     <row r="46">
       <c r="A46" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="B46" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="C46" s="2"/>
       <c r="D46" t="s" s="2">
-        <v>361</v>
+        <v>362</v>
       </c>
       <c r="E46" s="2"/>
       <c r="F46" t="s" s="2">
@@ -7494,13 +7497,13 @@
         <v>81</v>
       </c>
       <c r="K46" t="s" s="2">
-        <v>362</v>
+        <v>363</v>
       </c>
       <c r="L46" t="s" s="2">
-        <v>363</v>
+        <v>364</v>
       </c>
       <c r="M46" t="s" s="2">
-        <v>364</v>
+        <v>365</v>
       </c>
       <c r="N46" s="2"/>
       <c r="O46" s="2"/>
@@ -7551,7 +7554,7 @@
         <v>81</v>
       </c>
       <c r="AF46" t="s" s="2">
-        <v>360</v>
+        <v>361</v>
       </c>
       <c r="AG46" t="s" s="2">
         <v>79</v>
@@ -7569,10 +7572,10 @@
         <v>81</v>
       </c>
       <c r="AL46" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AM46" t="s" s="2">
-        <v>366</v>
+        <v>367</v>
       </c>
       <c r="AN46" t="s" s="2">
         <v>81</v>
@@ -7583,10 +7586,10 @@
     </row>
     <row r="47">
       <c r="A47" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="B47" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="C47" s="2"/>
       <c r="D47" t="s" s="2">
@@ -7609,13 +7612,13 @@
         <v>91</v>
       </c>
       <c r="K47" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L47" t="s" s="2">
-        <v>368</v>
+        <v>369</v>
       </c>
       <c r="M47" t="s" s="2">
-        <v>369</v>
+        <v>370</v>
       </c>
       <c r="N47" s="2"/>
       <c r="O47" s="2"/>
@@ -7666,7 +7669,7 @@
         <v>81</v>
       </c>
       <c r="AF47" t="s" s="2">
-        <v>367</v>
+        <v>368</v>
       </c>
       <c r="AG47" t="s" s="2">
         <v>79</v>
@@ -7684,24 +7687,24 @@
         <v>81</v>
       </c>
       <c r="AL47" t="s" s="2">
-        <v>370</v>
+        <v>371</v>
       </c>
       <c r="AM47" t="s" s="2">
-        <v>371</v>
+        <v>372</v>
       </c>
       <c r="AN47" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO47" t="s" s="2">
-        <v>372</v>
+        <v>373</v>
       </c>
     </row>
     <row r="48">
       <c r="A48" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="B48" t="s" s="2">
-        <v>373</v>
+        <v>374</v>
       </c>
       <c r="C48" s="2"/>
       <c r="D48" t="s" s="2">
@@ -7813,10 +7816,10 @@
     </row>
     <row r="49">
       <c r="A49" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="B49" t="s" s="2">
-        <v>374</v>
+        <v>375</v>
       </c>
       <c r="C49" s="2"/>
       <c r="D49" t="s" s="2">
@@ -7930,14 +7933,14 @@
     </row>
     <row r="50">
       <c r="A50" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="B50" t="s" s="2">
-        <v>375</v>
+        <v>376</v>
       </c>
       <c r="C50" s="2"/>
       <c r="D50" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E50" s="2"/>
       <c r="F50" t="s" s="2">
@@ -7959,10 +7962,10 @@
         <v>135</v>
       </c>
       <c r="L50" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M50" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N50" t="s" s="2">
         <v>183</v>
@@ -8017,7 +8020,7 @@
         <v>81</v>
       </c>
       <c r="AF50" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG50" t="s" s="2">
         <v>79</v>
@@ -8049,10 +8052,10 @@
     </row>
     <row r="51">
       <c r="A51" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="B51" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="C51" s="2"/>
       <c r="D51" t="s" s="2">
@@ -8078,13 +8081,13 @@
         <v>225</v>
       </c>
       <c r="L51" t="s" s="2">
-        <v>377</v>
+        <v>378</v>
       </c>
       <c r="M51" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="N51" t="s" s="2">
-        <v>379</v>
+        <v>380</v>
       </c>
       <c r="O51" s="2"/>
       <c r="P51" t="s" s="2">
@@ -8113,10 +8116,10 @@
         <v>231</v>
       </c>
       <c r="Y51" t="s" s="2">
-        <v>378</v>
+        <v>379</v>
       </c>
       <c r="Z51" t="s" s="2">
-        <v>380</v>
+        <v>381</v>
       </c>
       <c r="AA51" t="s" s="2">
         <v>81</v>
@@ -8134,7 +8137,7 @@
         <v>81</v>
       </c>
       <c r="AF51" t="s" s="2">
-        <v>376</v>
+        <v>377</v>
       </c>
       <c r="AG51" t="s" s="2">
         <v>79</v>
@@ -8152,24 +8155,24 @@
         <v>81</v>
       </c>
       <c r="AL51" t="s" s="2">
-        <v>381</v>
+        <v>382</v>
       </c>
       <c r="AM51" t="s" s="2">
-        <v>382</v>
+        <v>383</v>
       </c>
       <c r="AN51" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO51" t="s" s="2">
-        <v>383</v>
+        <v>384</v>
       </c>
     </row>
     <row r="52">
       <c r="A52" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="B52" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="C52" s="2"/>
       <c r="D52" t="s" s="2">
@@ -8192,13 +8195,13 @@
         <v>81</v>
       </c>
       <c r="K52" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L52" t="s" s="2">
-        <v>385</v>
+        <v>386</v>
       </c>
       <c r="M52" t="s" s="2">
-        <v>386</v>
+        <v>387</v>
       </c>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
@@ -8249,7 +8252,7 @@
         <v>81</v>
       </c>
       <c r="AF52" t="s" s="2">
-        <v>384</v>
+        <v>385</v>
       </c>
       <c r="AG52" t="s" s="2">
         <v>79</v>
@@ -8270,21 +8273,21 @@
         <v>81</v>
       </c>
       <c r="AM52" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AN52" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO52" t="s" s="2">
-        <v>388</v>
+        <v>389</v>
       </c>
     </row>
     <row r="53">
       <c r="A53" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="B53" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="C53" s="2"/>
       <c r="D53" t="s" s="2">
@@ -8307,13 +8310,13 @@
         <v>91</v>
       </c>
       <c r="K53" t="s" s="2">
-        <v>390</v>
+        <v>391</v>
       </c>
       <c r="L53" t="s" s="2">
-        <v>391</v>
+        <v>392</v>
       </c>
       <c r="M53" t="s" s="2">
-        <v>392</v>
+        <v>393</v>
       </c>
       <c r="N53" s="2"/>
       <c r="O53" s="2"/>
@@ -8364,7 +8367,7 @@
         <v>81</v>
       </c>
       <c r="AF53" t="s" s="2">
-        <v>389</v>
+        <v>390</v>
       </c>
       <c r="AG53" t="s" s="2">
         <v>79</v>
@@ -8382,24 +8385,24 @@
         <v>81</v>
       </c>
       <c r="AL53" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AM53" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AN53" t="s" s="2">
-        <v>395</v>
+        <v>396</v>
       </c>
       <c r="AO53" t="s" s="2">
-        <v>396</v>
+        <v>397</v>
       </c>
     </row>
     <row r="54">
       <c r="A54" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="B54" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="C54" s="2"/>
       <c r="D54" t="s" s="2">
@@ -8422,13 +8425,13 @@
         <v>91</v>
       </c>
       <c r="K54" t="s" s="2">
-        <v>398</v>
+        <v>399</v>
       </c>
       <c r="L54" t="s" s="2">
-        <v>399</v>
+        <v>400</v>
       </c>
       <c r="M54" t="s" s="2">
-        <v>400</v>
+        <v>401</v>
       </c>
       <c r="N54" s="2"/>
       <c r="O54" s="2"/>
@@ -8479,7 +8482,7 @@
         <v>81</v>
       </c>
       <c r="AF54" t="s" s="2">
-        <v>397</v>
+        <v>398</v>
       </c>
       <c r="AG54" t="s" s="2">
         <v>79</v>
@@ -8497,24 +8500,24 @@
         <v>81</v>
       </c>
       <c r="AL54" t="s" s="2">
-        <v>365</v>
+        <v>366</v>
       </c>
       <c r="AM54" t="s" s="2">
-        <v>401</v>
+        <v>402</v>
       </c>
       <c r="AN54" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO54" t="s" s="2">
-        <v>402</v>
+        <v>403</v>
       </c>
     </row>
     <row r="55">
       <c r="A55" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="B55" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="C55" s="2"/>
       <c r="D55" t="s" s="2">
@@ -8537,16 +8540,16 @@
         <v>81</v>
       </c>
       <c r="K55" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L55" t="s" s="2">
-        <v>404</v>
+        <v>405</v>
       </c>
       <c r="M55" t="s" s="2">
-        <v>405</v>
+        <v>406</v>
       </c>
       <c r="N55" t="s" s="2">
-        <v>406</v>
+        <v>407</v>
       </c>
       <c r="O55" s="2"/>
       <c r="P55" t="s" s="2">
@@ -8596,7 +8599,7 @@
         <v>81</v>
       </c>
       <c r="AF55" t="s" s="2">
-        <v>403</v>
+        <v>404</v>
       </c>
       <c r="AG55" t="s" s="2">
         <v>79</v>
@@ -8614,24 +8617,24 @@
         <v>81</v>
       </c>
       <c r="AL55" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AM55" t="s" s="2">
-        <v>408</v>
+        <v>409</v>
       </c>
       <c r="AN55" t="s" s="2">
-        <v>409</v>
+        <v>410</v>
       </c>
       <c r="AO55" t="s" s="2">
-        <v>410</v>
+        <v>411</v>
       </c>
     </row>
     <row r="56">
       <c r="A56" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="B56" t="s" s="2">
-        <v>411</v>
+        <v>412</v>
       </c>
       <c r="C56" s="2"/>
       <c r="D56" t="s" s="2">
@@ -8743,10 +8746,10 @@
     </row>
     <row r="57">
       <c r="A57" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="B57" t="s" s="2">
-        <v>412</v>
+        <v>413</v>
       </c>
       <c r="C57" s="2"/>
       <c r="D57" t="s" s="2">
@@ -8860,10 +8863,10 @@
     </row>
     <row r="58">
       <c r="A58" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="B58" t="s" s="2">
-        <v>413</v>
+        <v>414</v>
       </c>
       <c r="C58" s="2"/>
       <c r="D58" t="s" s="2">
@@ -8886,16 +8889,16 @@
         <v>91</v>
       </c>
       <c r="K58" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="L58" t="s" s="2">
-        <v>415</v>
+        <v>416</v>
       </c>
       <c r="M58" t="s" s="2">
-        <v>416</v>
+        <v>417</v>
       </c>
       <c r="N58" t="s" s="2">
-        <v>417</v>
+        <v>418</v>
       </c>
       <c r="O58" s="2"/>
       <c r="P58" t="s" s="2">
@@ -8945,7 +8948,7 @@
         <v>81</v>
       </c>
       <c r="AF58" t="s" s="2">
-        <v>418</v>
+        <v>419</v>
       </c>
       <c r="AG58" t="s" s="2">
         <v>79</v>
@@ -8954,33 +8957,33 @@
         <v>90</v>
       </c>
       <c r="AI58" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AJ58" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AK58" t="s" s="2">
-        <v>420</v>
+        <v>421</v>
       </c>
       <c r="AL58" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AM58" t="s" s="2">
-        <v>421</v>
+        <v>422</v>
       </c>
       <c r="AN58" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO58" t="s" s="2">
-        <v>422</v>
+        <v>423</v>
       </c>
     </row>
     <row r="59">
       <c r="A59" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="B59" t="s" s="2">
-        <v>423</v>
+        <v>424</v>
       </c>
       <c r="C59" s="2"/>
       <c r="D59" t="s" s="2">
@@ -9003,23 +9006,23 @@
         <v>91</v>
       </c>
       <c r="K59" t="s" s="2">
-        <v>414</v>
+        <v>415</v>
       </c>
       <c r="L59" t="s" s="2">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="M59" t="s" s="2">
-        <v>425</v>
+        <v>426</v>
       </c>
       <c r="N59" t="s" s="2">
-        <v>426</v>
+        <v>427</v>
       </c>
       <c r="O59" s="2"/>
       <c r="P59" t="s" s="2">
         <v>81</v>
       </c>
       <c r="Q59" t="s" s="2">
-        <v>427</v>
+        <v>428</v>
       </c>
       <c r="R59" t="s" s="2">
         <v>81</v>
@@ -9064,7 +9067,7 @@
         <v>81</v>
       </c>
       <c r="AF59" t="s" s="2">
-        <v>428</v>
+        <v>429</v>
       </c>
       <c r="AG59" t="s" s="2">
         <v>79</v>
@@ -9073,33 +9076,33 @@
         <v>90</v>
       </c>
       <c r="AI59" t="s" s="2">
-        <v>419</v>
+        <v>420</v>
       </c>
       <c r="AJ59" t="s" s="2">
         <v>102</v>
       </c>
       <c r="AK59" t="s" s="2">
-        <v>429</v>
+        <v>430</v>
       </c>
       <c r="AL59" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AM59" t="s" s="2">
-        <v>430</v>
+        <v>431</v>
       </c>
       <c r="AN59" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO59" t="s" s="2">
-        <v>431</v>
+        <v>432</v>
       </c>
     </row>
     <row r="60">
       <c r="A60" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="B60" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="C60" s="2"/>
       <c r="D60" t="s" s="2">
@@ -9122,16 +9125,16 @@
         <v>81</v>
       </c>
       <c r="K60" t="s" s="2">
-        <v>433</v>
+        <v>434</v>
       </c>
       <c r="L60" t="s" s="2">
-        <v>434</v>
+        <v>435</v>
       </c>
       <c r="M60" t="s" s="2">
-        <v>435</v>
+        <v>436</v>
       </c>
       <c r="N60" t="s" s="2">
-        <v>436</v>
+        <v>437</v>
       </c>
       <c r="O60" s="2"/>
       <c r="P60" t="s" s="2">
@@ -9181,7 +9184,7 @@
         <v>81</v>
       </c>
       <c r="AF60" t="s" s="2">
-        <v>432</v>
+        <v>433</v>
       </c>
       <c r="AG60" t="s" s="2">
         <v>79</v>
@@ -9199,28 +9202,28 @@
         <v>81</v>
       </c>
       <c r="AL60" t="s" s="2">
-        <v>407</v>
+        <v>408</v>
       </c>
       <c r="AM60" t="s" s="2">
-        <v>437</v>
+        <v>438</v>
       </c>
       <c r="AN60" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO60" t="s" s="2">
-        <v>438</v>
+        <v>439</v>
       </c>
     </row>
     <row r="61">
       <c r="A61" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="B61" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="C61" s="2"/>
       <c r="D61" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E61" s="2"/>
       <c r="F61" t="s" s="2">
@@ -9242,13 +9245,13 @@
         <v>225</v>
       </c>
       <c r="L61" t="s" s="2">
-        <v>441</v>
+        <v>442</v>
       </c>
       <c r="M61" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="N61" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="O61" s="2"/>
       <c r="P61" t="s" s="2">
@@ -9277,10 +9280,10 @@
         <v>114</v>
       </c>
       <c r="Y61" t="s" s="2">
-        <v>444</v>
+        <v>445</v>
       </c>
       <c r="Z61" t="s" s="2">
-        <v>445</v>
+        <v>446</v>
       </c>
       <c r="AA61" t="s" s="2">
         <v>81</v>
@@ -9298,7 +9301,7 @@
         <v>81</v>
       </c>
       <c r="AF61" t="s" s="2">
-        <v>439</v>
+        <v>440</v>
       </c>
       <c r="AG61" t="s" s="2">
         <v>79</v>
@@ -9316,28 +9319,28 @@
         <v>81</v>
       </c>
       <c r="AL61" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AM61" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AN61" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AO61" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="62">
       <c r="A62" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="B62" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="C62" s="2"/>
       <c r="D62" t="s" s="2">
-        <v>440</v>
+        <v>441</v>
       </c>
       <c r="E62" s="2"/>
       <c r="F62" t="s" s="2">
@@ -9356,16 +9359,16 @@
         <v>91</v>
       </c>
       <c r="K62" t="s" s="2">
-        <v>451</v>
+        <v>452</v>
       </c>
       <c r="L62" t="s" s="2">
-        <v>452</v>
+        <v>453</v>
       </c>
       <c r="M62" t="s" s="2">
-        <v>442</v>
+        <v>443</v>
       </c>
       <c r="N62" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="O62" s="2"/>
       <c r="P62" t="s" s="2">
@@ -9415,7 +9418,7 @@
         <v>81</v>
       </c>
       <c r="AF62" t="s" s="2">
-        <v>450</v>
+        <v>451</v>
       </c>
       <c r="AG62" t="s" s="2">
         <v>79</v>
@@ -9433,24 +9436,24 @@
         <v>81</v>
       </c>
       <c r="AL62" t="s" s="2">
-        <v>446</v>
+        <v>447</v>
       </c>
       <c r="AM62" t="s" s="2">
-        <v>447</v>
+        <v>448</v>
       </c>
       <c r="AN62" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AO62" t="s" s="2">
-        <v>449</v>
+        <v>450</v>
       </c>
     </row>
     <row r="63">
       <c r="A63" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="B63" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="C63" s="2"/>
       <c r="D63" t="s" s="2">
@@ -9473,13 +9476,13 @@
         <v>91</v>
       </c>
       <c r="K63" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L63" t="s" s="2">
-        <v>454</v>
+        <v>455</v>
       </c>
       <c r="M63" t="s" s="2">
-        <v>455</v>
+        <v>456</v>
       </c>
       <c r="N63" s="2"/>
       <c r="O63" s="2"/>
@@ -9530,7 +9533,7 @@
         <v>81</v>
       </c>
       <c r="AF63" t="s" s="2">
-        <v>453</v>
+        <v>454</v>
       </c>
       <c r="AG63" t="s" s="2">
         <v>79</v>
@@ -9551,7 +9554,7 @@
         <v>81</v>
       </c>
       <c r="AM63" t="s" s="2">
-        <v>456</v>
+        <v>457</v>
       </c>
       <c r="AN63" t="s" s="2">
         <v>81</v>
@@ -9562,10 +9565,10 @@
     </row>
     <row r="64">
       <c r="A64" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="B64" t="s" s="2">
-        <v>457</v>
+        <v>458</v>
       </c>
       <c r="C64" s="2"/>
       <c r="D64" t="s" s="2">
@@ -9677,10 +9680,10 @@
     </row>
     <row r="65">
       <c r="A65" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="B65" t="s" s="2">
-        <v>458</v>
+        <v>459</v>
       </c>
       <c r="C65" s="2"/>
       <c r="D65" t="s" s="2">
@@ -9794,14 +9797,14 @@
     </row>
     <row r="66">
       <c r="A66" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="B66" t="s" s="2">
-        <v>459</v>
+        <v>460</v>
       </c>
       <c r="C66" s="2"/>
       <c r="D66" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E66" s="2"/>
       <c r="F66" t="s" s="2">
@@ -9823,10 +9826,10 @@
         <v>135</v>
       </c>
       <c r="L66" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M66" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N66" t="s" s="2">
         <v>183</v>
@@ -9881,7 +9884,7 @@
         <v>81</v>
       </c>
       <c r="AF66" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG66" t="s" s="2">
         <v>79</v>
@@ -9913,14 +9916,14 @@
     </row>
     <row r="67">
       <c r="A67" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="B67" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="C67" s="2"/>
       <c r="D67" t="s" s="2">
-        <v>461</v>
+        <v>462</v>
       </c>
       <c r="E67" s="2"/>
       <c r="F67" t="s" s="2">
@@ -9939,16 +9942,16 @@
         <v>91</v>
       </c>
       <c r="K67" t="s" s="2">
-        <v>462</v>
+        <v>463</v>
       </c>
       <c r="L67" t="s" s="2">
-        <v>463</v>
+        <v>464</v>
       </c>
       <c r="M67" t="s" s="2">
-        <v>464</v>
+        <v>465</v>
       </c>
       <c r="N67" t="s" s="2">
-        <v>443</v>
+        <v>444</v>
       </c>
       <c r="O67" s="2"/>
       <c r="P67" t="s" s="2">
@@ -9998,7 +10001,7 @@
         <v>81</v>
       </c>
       <c r="AF67" t="s" s="2">
-        <v>460</v>
+        <v>461</v>
       </c>
       <c r="AG67" t="s" s="2">
         <v>90</v>
@@ -10016,24 +10019,24 @@
         <v>81</v>
       </c>
       <c r="AL67" t="s" s="2">
-        <v>465</v>
+        <v>466</v>
       </c>
       <c r="AM67" t="s" s="2">
-        <v>466</v>
+        <v>467</v>
       </c>
       <c r="AN67" t="s" s="2">
-        <v>448</v>
+        <v>449</v>
       </c>
       <c r="AO67" t="s" s="2">
-        <v>467</v>
+        <v>468</v>
       </c>
     </row>
     <row r="68">
       <c r="A68" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="B68" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="C68" s="2"/>
       <c r="D68" t="s" s="2">
@@ -10059,10 +10062,10 @@
         <v>225</v>
       </c>
       <c r="L68" t="s" s="2">
-        <v>469</v>
+        <v>470</v>
       </c>
       <c r="M68" t="s" s="2">
-        <v>470</v>
+        <v>471</v>
       </c>
       <c r="N68" s="2"/>
       <c r="O68" s="2"/>
@@ -10092,10 +10095,10 @@
         <v>114</v>
       </c>
       <c r="Y68" t="s" s="2">
-        <v>471</v>
+        <v>472</v>
       </c>
       <c r="Z68" t="s" s="2">
-        <v>472</v>
+        <v>473</v>
       </c>
       <c r="AA68" t="s" s="2">
         <v>81</v>
@@ -10113,7 +10116,7 @@
         <v>81</v>
       </c>
       <c r="AF68" t="s" s="2">
-        <v>468</v>
+        <v>469</v>
       </c>
       <c r="AG68" t="s" s="2">
         <v>79</v>
@@ -10145,10 +10148,10 @@
     </row>
     <row r="69">
       <c r="A69" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="B69" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="C69" s="2"/>
       <c r="D69" t="s" s="2">
@@ -10171,13 +10174,13 @@
         <v>81</v>
       </c>
       <c r="K69" t="s" s="2">
-        <v>474</v>
+        <v>475</v>
       </c>
       <c r="L69" t="s" s="2">
-        <v>475</v>
+        <v>476</v>
       </c>
       <c r="M69" t="s" s="2">
-        <v>476</v>
+        <v>477</v>
       </c>
       <c r="N69" s="2"/>
       <c r="O69" s="2"/>
@@ -10228,7 +10231,7 @@
         <v>81</v>
       </c>
       <c r="AF69" t="s" s="2">
-        <v>473</v>
+        <v>474</v>
       </c>
       <c r="AG69" t="s" s="2">
         <v>79</v>
@@ -10249,7 +10252,7 @@
         <v>81</v>
       </c>
       <c r="AM69" t="s" s="2">
-        <v>477</v>
+        <v>478</v>
       </c>
       <c r="AN69" t="s" s="2">
         <v>81</v>
@@ -10260,10 +10263,10 @@
     </row>
     <row r="70">
       <c r="A70" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="B70" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="C70" s="2"/>
       <c r="D70" t="s" s="2">
@@ -10286,16 +10289,16 @@
         <v>81</v>
       </c>
       <c r="K70" t="s" s="2">
-        <v>479</v>
+        <v>480</v>
       </c>
       <c r="L70" t="s" s="2">
-        <v>480</v>
+        <v>481</v>
       </c>
       <c r="M70" t="s" s="2">
-        <v>481</v>
+        <v>482</v>
       </c>
       <c r="N70" t="s" s="2">
-        <v>482</v>
+        <v>483</v>
       </c>
       <c r="O70" s="2"/>
       <c r="P70" t="s" s="2">
@@ -10345,7 +10348,7 @@
         <v>81</v>
       </c>
       <c r="AF70" t="s" s="2">
-        <v>478</v>
+        <v>479</v>
       </c>
       <c r="AG70" t="s" s="2">
         <v>79</v>
@@ -10366,7 +10369,7 @@
         <v>81</v>
       </c>
       <c r="AM70" t="s" s="2">
-        <v>483</v>
+        <v>484</v>
       </c>
       <c r="AN70" t="s" s="2">
         <v>81</v>
@@ -10377,10 +10380,10 @@
     </row>
     <row r="71">
       <c r="A71" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="B71" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="C71" s="2"/>
       <c r="D71" t="s" s="2">
@@ -10403,16 +10406,16 @@
         <v>81</v>
       </c>
       <c r="K71" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L71" t="s" s="2">
-        <v>485</v>
+        <v>486</v>
       </c>
       <c r="M71" t="s" s="2">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="N71" t="s" s="2">
-        <v>487</v>
+        <v>488</v>
       </c>
       <c r="O71" s="2"/>
       <c r="P71" t="s" s="2">
@@ -10462,7 +10465,7 @@
         <v>81</v>
       </c>
       <c r="AF71" t="s" s="2">
-        <v>484</v>
+        <v>485</v>
       </c>
       <c r="AG71" t="s" s="2">
         <v>79</v>
@@ -10483,7 +10486,7 @@
         <v>81</v>
       </c>
       <c r="AM71" t="s" s="2">
-        <v>488</v>
+        <v>489</v>
       </c>
       <c r="AN71" t="s" s="2">
         <v>81</v>
@@ -10494,10 +10497,10 @@
     </row>
     <row r="72">
       <c r="A72" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="B72" t="s" s="2">
-        <v>489</v>
+        <v>490</v>
       </c>
       <c r="C72" s="2"/>
       <c r="D72" t="s" s="2">
@@ -10609,10 +10612,10 @@
     </row>
     <row r="73">
       <c r="A73" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="B73" t="s" s="2">
-        <v>490</v>
+        <v>491</v>
       </c>
       <c r="C73" s="2"/>
       <c r="D73" t="s" s="2">
@@ -10726,14 +10729,14 @@
     </row>
     <row r="74">
       <c r="A74" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="B74" t="s" s="2">
-        <v>491</v>
+        <v>492</v>
       </c>
       <c r="C74" s="2"/>
       <c r="D74" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E74" s="2"/>
       <c r="F74" t="s" s="2">
@@ -10755,10 +10758,10 @@
         <v>135</v>
       </c>
       <c r="L74" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M74" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N74" t="s" s="2">
         <v>183</v>
@@ -10813,7 +10816,7 @@
         <v>81</v>
       </c>
       <c r="AF74" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG74" t="s" s="2">
         <v>79</v>
@@ -10845,10 +10848,10 @@
     </row>
     <row r="75">
       <c r="A75" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="B75" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="C75" s="2"/>
       <c r="D75" t="s" s="2">
@@ -10874,10 +10877,10 @@
         <v>187</v>
       </c>
       <c r="L75" t="s" s="2">
-        <v>493</v>
+        <v>494</v>
       </c>
       <c r="M75" t="s" s="2">
-        <v>494</v>
+        <v>495</v>
       </c>
       <c r="N75" s="2"/>
       <c r="O75" s="2"/>
@@ -10928,7 +10931,7 @@
         <v>81</v>
       </c>
       <c r="AF75" t="s" s="2">
-        <v>492</v>
+        <v>493</v>
       </c>
       <c r="AG75" t="s" s="2">
         <v>79</v>
@@ -10955,15 +10958,15 @@
         <v>81</v>
       </c>
       <c r="AO75" t="s" s="2">
-        <v>495</v>
+        <v>496</v>
       </c>
     </row>
     <row r="76">
       <c r="A76" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="B76" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="C76" s="2"/>
       <c r="D76" t="s" s="2">
@@ -10986,13 +10989,13 @@
         <v>81</v>
       </c>
       <c r="K76" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="L76" t="s" s="2">
-        <v>498</v>
+        <v>499</v>
       </c>
       <c r="M76" t="s" s="2">
-        <v>499</v>
+        <v>500</v>
       </c>
       <c r="N76" s="2"/>
       <c r="O76" s="2"/>
@@ -11043,7 +11046,7 @@
         <v>81</v>
       </c>
       <c r="AF76" t="s" s="2">
-        <v>496</v>
+        <v>497</v>
       </c>
       <c r="AG76" t="s" s="2">
         <v>79</v>
@@ -11064,7 +11067,7 @@
         <v>81</v>
       </c>
       <c r="AM76" t="s" s="2">
-        <v>500</v>
+        <v>501</v>
       </c>
       <c r="AN76" t="s" s="2">
         <v>81</v>
@@ -11075,10 +11078,10 @@
     </row>
     <row r="77">
       <c r="A77" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="B77" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="C77" s="2"/>
       <c r="D77" t="s" s="2">
@@ -11104,10 +11107,10 @@
         <v>225</v>
       </c>
       <c r="L77" t="s" s="2">
-        <v>502</v>
+        <v>503</v>
       </c>
       <c r="M77" t="s" s="2">
-        <v>503</v>
+        <v>504</v>
       </c>
       <c r="N77" s="2"/>
       <c r="O77" s="2"/>
@@ -11137,10 +11140,10 @@
         <v>114</v>
       </c>
       <c r="Y77" t="s" s="2">
-        <v>504</v>
+        <v>505</v>
       </c>
       <c r="Z77" t="s" s="2">
-        <v>505</v>
+        <v>506</v>
       </c>
       <c r="AA77" t="s" s="2">
         <v>81</v>
@@ -11158,7 +11161,7 @@
         <v>81</v>
       </c>
       <c r="AF77" t="s" s="2">
-        <v>501</v>
+        <v>502</v>
       </c>
       <c r="AG77" t="s" s="2">
         <v>79</v>
@@ -11179,21 +11182,21 @@
         <v>81</v>
       </c>
       <c r="AM77" t="s" s="2">
-        <v>506</v>
+        <v>507</v>
       </c>
       <c r="AN77" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO77" t="s" s="2">
-        <v>507</v>
+        <v>508</v>
       </c>
     </row>
     <row r="78">
       <c r="A78" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="B78" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="C78" s="2"/>
       <c r="D78" t="s" s="2">
@@ -11219,10 +11222,10 @@
         <v>225</v>
       </c>
       <c r="L78" t="s" s="2">
-        <v>509</v>
+        <v>510</v>
       </c>
       <c r="M78" t="s" s="2">
-        <v>510</v>
+        <v>511</v>
       </c>
       <c r="N78" s="2"/>
       <c r="O78" s="2"/>
@@ -11249,13 +11252,13 @@
         <v>81</v>
       </c>
       <c r="X78" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Y78" t="s" s="2">
-        <v>511</v>
+        <v>512</v>
       </c>
       <c r="Z78" t="s" s="2">
-        <v>512</v>
+        <v>513</v>
       </c>
       <c r="AA78" t="s" s="2">
         <v>81</v>
@@ -11273,7 +11276,7 @@
         <v>81</v>
       </c>
       <c r="AF78" t="s" s="2">
-        <v>508</v>
+        <v>509</v>
       </c>
       <c r="AG78" t="s" s="2">
         <v>79</v>
@@ -11300,15 +11303,15 @@
         <v>81</v>
       </c>
       <c r="AO78" t="s" s="2">
-        <v>513</v>
+        <v>514</v>
       </c>
     </row>
     <row r="79">
       <c r="A79" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="B79" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="C79" s="2"/>
       <c r="D79" t="s" s="2">
@@ -11334,16 +11337,16 @@
         <v>225</v>
       </c>
       <c r="L79" t="s" s="2">
-        <v>515</v>
+        <v>516</v>
       </c>
       <c r="M79" t="s" s="2">
-        <v>516</v>
+        <v>517</v>
       </c>
       <c r="N79" t="s" s="2">
-        <v>517</v>
+        <v>518</v>
       </c>
       <c r="O79" t="s" s="2">
-        <v>518</v>
+        <v>519</v>
       </c>
       <c r="P79" t="s" s="2">
         <v>81</v>
@@ -11368,13 +11371,13 @@
         <v>81</v>
       </c>
       <c r="X79" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Y79" t="s" s="2">
-        <v>519</v>
+        <v>520</v>
       </c>
       <c r="Z79" t="s" s="2">
-        <v>520</v>
+        <v>521</v>
       </c>
       <c r="AA79" t="s" s="2">
         <v>81</v>
@@ -11392,7 +11395,7 @@
         <v>81</v>
       </c>
       <c r="AF79" t="s" s="2">
-        <v>514</v>
+        <v>515</v>
       </c>
       <c r="AG79" t="s" s="2">
         <v>79</v>
@@ -11413,21 +11416,21 @@
         <v>81</v>
       </c>
       <c r="AM79" t="s" s="2">
-        <v>521</v>
+        <v>522</v>
       </c>
       <c r="AN79" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO79" t="s" s="2">
-        <v>522</v>
+        <v>523</v>
       </c>
     </row>
     <row r="80">
       <c r="A80" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="B80" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="C80" s="2"/>
       <c r="D80" t="s" s="2">
@@ -11453,10 +11456,10 @@
         <v>225</v>
       </c>
       <c r="L80" t="s" s="2">
-        <v>524</v>
+        <v>525</v>
       </c>
       <c r="M80" t="s" s="2">
-        <v>525</v>
+        <v>526</v>
       </c>
       <c r="N80" s="2"/>
       <c r="O80" s="2"/>
@@ -11486,10 +11489,10 @@
         <v>114</v>
       </c>
       <c r="Y80" t="s" s="2">
-        <v>526</v>
+        <v>527</v>
       </c>
       <c r="Z80" t="s" s="2">
-        <v>527</v>
+        <v>528</v>
       </c>
       <c r="AA80" t="s" s="2">
         <v>81</v>
@@ -11507,7 +11510,7 @@
         <v>81</v>
       </c>
       <c r="AF80" t="s" s="2">
-        <v>523</v>
+        <v>524</v>
       </c>
       <c r="AG80" t="s" s="2">
         <v>79</v>
@@ -11528,21 +11531,21 @@
         <v>81</v>
       </c>
       <c r="AM80" t="s" s="2">
-        <v>528</v>
+        <v>529</v>
       </c>
       <c r="AN80" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO80" t="s" s="2">
-        <v>529</v>
+        <v>530</v>
       </c>
     </row>
     <row r="81">
       <c r="A81" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="B81" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="C81" s="2"/>
       <c r="D81" t="s" s="2">
@@ -11568,10 +11571,10 @@
         <v>225</v>
       </c>
       <c r="L81" t="s" s="2">
-        <v>531</v>
+        <v>532</v>
       </c>
       <c r="M81" t="s" s="2">
-        <v>532</v>
+        <v>533</v>
       </c>
       <c r="N81" s="2"/>
       <c r="O81" s="2"/>
@@ -11601,10 +11604,10 @@
         <v>114</v>
       </c>
       <c r="Y81" t="s" s="2">
-        <v>533</v>
+        <v>534</v>
       </c>
       <c r="Z81" t="s" s="2">
-        <v>534</v>
+        <v>535</v>
       </c>
       <c r="AA81" t="s" s="2">
         <v>81</v>
@@ -11622,7 +11625,7 @@
         <v>81</v>
       </c>
       <c r="AF81" t="s" s="2">
-        <v>530</v>
+        <v>531</v>
       </c>
       <c r="AG81" t="s" s="2">
         <v>79</v>
@@ -11643,21 +11646,21 @@
         <v>81</v>
       </c>
       <c r="AM81" t="s" s="2">
-        <v>535</v>
+        <v>536</v>
       </c>
       <c r="AN81" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO81" t="s" s="2">
-        <v>536</v>
+        <v>537</v>
       </c>
     </row>
     <row r="82">
       <c r="A82" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="B82" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="C82" s="2"/>
       <c r="D82" t="s" s="2">
@@ -11680,13 +11683,13 @@
         <v>81</v>
       </c>
       <c r="K82" t="s" s="2">
-        <v>497</v>
+        <v>498</v>
       </c>
       <c r="L82" t="s" s="2">
-        <v>538</v>
+        <v>539</v>
       </c>
       <c r="M82" t="s" s="2">
-        <v>539</v>
+        <v>540</v>
       </c>
       <c r="N82" s="2"/>
       <c r="O82" s="2"/>
@@ -11737,7 +11740,7 @@
         <v>81</v>
       </c>
       <c r="AF82" t="s" s="2">
-        <v>537</v>
+        <v>538</v>
       </c>
       <c r="AG82" t="s" s="2">
         <v>79</v>
@@ -11758,21 +11761,21 @@
         <v>81</v>
       </c>
       <c r="AM82" t="s" s="2">
-        <v>540</v>
+        <v>541</v>
       </c>
       <c r="AN82" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO82" t="s" s="2">
-        <v>541</v>
+        <v>542</v>
       </c>
     </row>
     <row r="83">
       <c r="A83" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="B83" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="C83" s="2"/>
       <c r="D83" t="s" s="2">
@@ -11798,10 +11801,10 @@
         <v>225</v>
       </c>
       <c r="L83" t="s" s="2">
-        <v>543</v>
+        <v>544</v>
       </c>
       <c r="M83" t="s" s="2">
-        <v>544</v>
+        <v>545</v>
       </c>
       <c r="N83" s="2"/>
       <c r="O83" s="2"/>
@@ -11828,13 +11831,13 @@
         <v>81</v>
       </c>
       <c r="X83" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Y83" t="s" s="2">
-        <v>545</v>
+        <v>546</v>
       </c>
       <c r="Z83" t="s" s="2">
-        <v>546</v>
+        <v>547</v>
       </c>
       <c r="AA83" t="s" s="2">
         <v>81</v>
@@ -11852,7 +11855,7 @@
         <v>81</v>
       </c>
       <c r="AF83" t="s" s="2">
-        <v>542</v>
+        <v>543</v>
       </c>
       <c r="AG83" t="s" s="2">
         <v>79</v>
@@ -11873,21 +11876,21 @@
         <v>81</v>
       </c>
       <c r="AM83" t="s" s="2">
-        <v>547</v>
+        <v>548</v>
       </c>
       <c r="AN83" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO83" t="s" s="2">
-        <v>548</v>
+        <v>549</v>
       </c>
     </row>
     <row r="84">
       <c r="A84" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="B84" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="C84" s="2"/>
       <c r="D84" t="s" s="2">
@@ -11910,16 +11913,16 @@
         <v>81</v>
       </c>
       <c r="K84" t="s" s="2">
-        <v>283</v>
+        <v>284</v>
       </c>
       <c r="L84" t="s" s="2">
-        <v>550</v>
+        <v>551</v>
       </c>
       <c r="M84" t="s" s="2">
-        <v>551</v>
+        <v>552</v>
       </c>
       <c r="N84" t="s" s="2">
-        <v>552</v>
+        <v>553</v>
       </c>
       <c r="O84" s="2"/>
       <c r="P84" t="s" s="2">
@@ -11969,7 +11972,7 @@
         <v>81</v>
       </c>
       <c r="AF84" t="s" s="2">
-        <v>549</v>
+        <v>550</v>
       </c>
       <c r="AG84" t="s" s="2">
         <v>79</v>
@@ -11990,7 +11993,7 @@
         <v>81</v>
       </c>
       <c r="AM84" t="s" s="2">
-        <v>553</v>
+        <v>554</v>
       </c>
       <c r="AN84" t="s" s="2">
         <v>81</v>
@@ -12001,10 +12004,10 @@
     </row>
     <row r="85">
       <c r="A85" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="B85" t="s" s="2">
-        <v>554</v>
+        <v>555</v>
       </c>
       <c r="C85" s="2"/>
       <c r="D85" t="s" s="2">
@@ -12116,10 +12119,10 @@
     </row>
     <row r="86">
       <c r="A86" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="B86" t="s" s="2">
-        <v>555</v>
+        <v>556</v>
       </c>
       <c r="C86" s="2"/>
       <c r="D86" t="s" s="2">
@@ -12233,14 +12236,14 @@
     </row>
     <row r="87">
       <c r="A87" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="B87" t="s" s="2">
-        <v>556</v>
+        <v>557</v>
       </c>
       <c r="C87" s="2"/>
       <c r="D87" t="s" s="2">
-        <v>290</v>
+        <v>291</v>
       </c>
       <c r="E87" s="2"/>
       <c r="F87" t="s" s="2">
@@ -12262,10 +12265,10 @@
         <v>135</v>
       </c>
       <c r="L87" t="s" s="2">
-        <v>291</v>
+        <v>292</v>
       </c>
       <c r="M87" t="s" s="2">
-        <v>292</v>
+        <v>293</v>
       </c>
       <c r="N87" t="s" s="2">
         <v>183</v>
@@ -12320,7 +12323,7 @@
         <v>81</v>
       </c>
       <c r="AF87" t="s" s="2">
-        <v>293</v>
+        <v>294</v>
       </c>
       <c r="AG87" t="s" s="2">
         <v>79</v>
@@ -12352,10 +12355,10 @@
     </row>
     <row r="88">
       <c r="A88" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="B88" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="C88" s="2"/>
       <c r="D88" t="s" s="2">
@@ -12378,13 +12381,13 @@
         <v>81</v>
       </c>
       <c r="K88" t="s" s="2">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="L88" t="s" s="2">
-        <v>559</v>
+        <v>560</v>
       </c>
       <c r="M88" t="s" s="2">
-        <v>560</v>
+        <v>561</v>
       </c>
       <c r="N88" s="2"/>
       <c r="O88" s="2"/>
@@ -12435,7 +12438,7 @@
         <v>81</v>
       </c>
       <c r="AF88" t="s" s="2">
-        <v>557</v>
+        <v>558</v>
       </c>
       <c r="AG88" t="s" s="2">
         <v>90</v>
@@ -12453,24 +12456,24 @@
         <v>81</v>
       </c>
       <c r="AL88" t="s" s="2">
-        <v>561</v>
+        <v>562</v>
       </c>
       <c r="AM88" t="s" s="2">
-        <v>394</v>
+        <v>395</v>
       </c>
       <c r="AN88" t="s" s="2">
-        <v>562</v>
+        <v>563</v>
       </c>
       <c r="AO88" t="s" s="2">
-        <v>563</v>
+        <v>564</v>
       </c>
     </row>
     <row r="89">
       <c r="A89" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="B89" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="C89" s="2"/>
       <c r="D89" t="s" s="2">
@@ -12496,13 +12499,13 @@
         <v>110</v>
       </c>
       <c r="L89" t="s" s="2">
-        <v>565</v>
+        <v>566</v>
       </c>
       <c r="M89" t="s" s="2">
-        <v>566</v>
+        <v>567</v>
       </c>
       <c r="N89" t="s" s="2">
-        <v>567</v>
+        <v>568</v>
       </c>
       <c r="O89" s="2"/>
       <c r="P89" t="s" s="2">
@@ -12531,10 +12534,10 @@
         <v>218</v>
       </c>
       <c r="Y89" t="s" s="2">
-        <v>568</v>
+        <v>569</v>
       </c>
       <c r="Z89" t="s" s="2">
-        <v>569</v>
+        <v>570</v>
       </c>
       <c r="AA89" t="s" s="2">
         <v>81</v>
@@ -12552,7 +12555,7 @@
         <v>81</v>
       </c>
       <c r="AF89" t="s" s="2">
-        <v>564</v>
+        <v>565</v>
       </c>
       <c r="AG89" t="s" s="2">
         <v>79</v>
@@ -12573,7 +12576,7 @@
         <v>81</v>
       </c>
       <c r="AM89" t="s" s="2">
-        <v>570</v>
+        <v>571</v>
       </c>
       <c r="AN89" t="s" s="2">
         <v>81</v>
@@ -12584,10 +12587,10 @@
     </row>
     <row r="90">
       <c r="A90" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="B90" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="C90" s="2"/>
       <c r="D90" t="s" s="2">
@@ -12613,13 +12616,13 @@
         <v>225</v>
       </c>
       <c r="L90" t="s" s="2">
-        <v>572</v>
+        <v>573</v>
       </c>
       <c r="M90" t="s" s="2">
-        <v>573</v>
+        <v>574</v>
       </c>
       <c r="N90" t="s" s="2">
-        <v>574</v>
+        <v>575</v>
       </c>
       <c r="O90" s="2"/>
       <c r="P90" t="s" s="2">
@@ -12645,13 +12648,13 @@
         <v>81</v>
       </c>
       <c r="X90" t="s" s="2">
-        <v>323</v>
+        <v>324</v>
       </c>
       <c r="Y90" t="s" s="2">
-        <v>575</v>
+        <v>576</v>
       </c>
       <c r="Z90" t="s" s="2">
-        <v>576</v>
+        <v>577</v>
       </c>
       <c r="AA90" t="s" s="2">
         <v>81</v>
@@ -12669,7 +12672,7 @@
         <v>81</v>
       </c>
       <c r="AF90" t="s" s="2">
-        <v>571</v>
+        <v>572</v>
       </c>
       <c r="AG90" t="s" s="2">
         <v>79</v>
@@ -12701,10 +12704,10 @@
     </row>
     <row r="91">
       <c r="A91" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="B91" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="C91" s="2"/>
       <c r="D91" t="s" s="2">
@@ -12727,13 +12730,13 @@
         <v>81</v>
       </c>
       <c r="K91" t="s" s="2">
-        <v>257</v>
+        <v>258</v>
       </c>
       <c r="L91" t="s" s="2">
-        <v>578</v>
+        <v>579</v>
       </c>
       <c r="M91" t="s" s="2">
-        <v>579</v>
+        <v>580</v>
       </c>
       <c r="N91" s="2"/>
       <c r="O91" s="2"/>
@@ -12784,7 +12787,7 @@
         <v>81</v>
       </c>
       <c r="AF91" t="s" s="2">
-        <v>577</v>
+        <v>578</v>
       </c>
       <c r="AG91" t="s" s="2">
         <v>79</v>
@@ -12805,7 +12808,7 @@
         <v>81</v>
       </c>
       <c r="AM91" t="s" s="2">
-        <v>387</v>
+        <v>388</v>
       </c>
       <c r="AN91" t="s" s="2">
         <v>81</v>
@@ -12816,10 +12819,10 @@
     </row>
     <row r="92">
       <c r="A92" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="B92" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="C92" s="2"/>
       <c r="D92" t="s" s="2">
@@ -12842,13 +12845,13 @@
         <v>81</v>
       </c>
       <c r="K92" t="s" s="2">
-        <v>581</v>
+        <v>582</v>
       </c>
       <c r="L92" t="s" s="2">
-        <v>582</v>
+        <v>583</v>
       </c>
       <c r="M92" t="s" s="2">
-        <v>583</v>
+        <v>584</v>
       </c>
       <c r="N92" s="2"/>
       <c r="O92" s="2"/>
@@ -12899,7 +12902,7 @@
         <v>81</v>
       </c>
       <c r="AF92" t="s" s="2">
-        <v>580</v>
+        <v>581</v>
       </c>
       <c r="AG92" t="s" s="2">
         <v>79</v>
@@ -12914,27 +12917,27 @@
         <v>102</v>
       </c>
       <c r="AK92" t="s" s="2">
-        <v>584</v>
+        <v>585</v>
       </c>
       <c r="AL92" t="s" s="2">
-        <v>393</v>
+        <v>394</v>
       </c>
       <c r="AM92" t="s" s="2">
-        <v>585</v>
+        <v>586</v>
       </c>
       <c r="AN92" t="s" s="2">
         <v>81</v>
       </c>
       <c r="AO92" t="s" s="2">
-        <v>586</v>
+        <v>587</v>
       </c>
     </row>
     <row r="93">
       <c r="A93" t="s" s="2">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="B93" t="s" s="2">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="C93" s="2"/>
       <c r="D93" t="s" s="2">
@@ -12957,16 +12960,16 @@
         <v>81</v>
       </c>
       <c r="K93" t="s" s="2">
-        <v>588</v>
+        <v>589</v>
       </c>
       <c r="L93" t="s" s="2">
-        <v>589</v>
+        <v>590</v>
       </c>
       <c r="M93" t="s" s="2">
-        <v>590</v>
+        <v>591</v>
       </c>
       <c r="N93" t="s" s="2">
-        <v>591</v>
+        <v>592</v>
       </c>
       <c r="O93" s="2"/>
       <c r="P93" t="s" s="2">
@@ -13016,7 +13019,7 @@
         <v>81</v>
       </c>
       <c r="AF93" t="s" s="2">
-        <v>587</v>
+        <v>588</v>
       </c>
       <c r="AG93" t="s" s="2">
         <v>79</v>
@@ -13034,10 +13037,10 @@
         <v>81</v>
       </c>
       <c r="AL93" t="s" s="2">
-        <v>592</v>
+        <v>593</v>
       </c>
       <c r="AM93" t="s" s="2">
-        <v>593</v>
+        <v>594</v>
       </c>
       <c r="AN93" t="s" s="2">
         <v>81</v>

</xml_diff>